<commit_message>
Updated the containers to be looked into, so that the process flows properly
</commit_message>
<xml_diff>
--- a/idnumber.xlsx
+++ b/idnumber.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28405"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DellUser\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DellUser\PycharmProjects\GovScrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{773151A0-D4AA-4186-B8AE-F00AB37A04A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75558A57-AD59-485C-819B-C64F6768AE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="2160" windowWidth="21600" windowHeight="11835" xr2:uid="{9497E6FA-E814-49A5-9D9A-888DE720C8A5}"/>
+    <workbookView xWindow="-23820" yWindow="1320" windowWidth="21570" windowHeight="11820" xr2:uid="{9497E6FA-E814-49A5-9D9A-888DE720C8A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D9B6E7-1BB5-4312-BAD7-4FA695E51661}">
   <dimension ref="A1:A119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>